<commit_message>
changed shortcuts to Ctrl/Cmd+N|O|S|Q
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="40" windowWidth="19980" windowHeight="27140" tabRatio="500"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="19980" windowHeight="27140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
   <si>
     <t>Shortcut</t>
   </si>
@@ -30,6 +30,9 @@
     <t xml:space="preserve">Context menu </t>
   </si>
   <si>
+    <t>Select new</t>
+  </si>
+  <si>
     <t>Left drag</t>
   </si>
   <si>
@@ -42,6 +45,9 @@
     <t>Shift right drag</t>
   </si>
   <si>
+    <t>Middle drag</t>
+  </si>
+  <si>
     <t>Make new object</t>
   </si>
   <si>
@@ -57,6 +63,9 @@
     <t>Double click object in Sidebar</t>
   </si>
   <si>
+    <t>Pick one peak at position</t>
+  </si>
+  <si>
     <t>Move module</t>
   </si>
   <si>
@@ -106,6 +115,30 @@
   </si>
   <si>
     <t xml:space="preserve">Set up NmrResidues </t>
+  </si>
+  <si>
+    <r>
+      <t>Zoom in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t xml:space="preserve">to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t>area</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -123,6 +156,48 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t>Add</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t>/Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t xml:space="preserve"> one to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t xml:space="preserve">/from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t>Selection</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Ctrl/Cmd+Z</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -297,22 +372,10 @@
     <t>Load Data</t>
   </si>
   <si>
-    <t>PN</t>
-  </si>
-  <si>
-    <t>PO</t>
-  </si>
-  <si>
     <t>LD</t>
   </si>
   <si>
-    <t>PS</t>
-  </si>
-  <si>
     <t>SA</t>
-  </si>
-  <si>
-    <t>QT</t>
   </si>
   <si>
     <t>ND</t>
@@ -628,33 +691,16 @@
     <t>W0, W1, …W9</t>
   </si>
   <si>
-    <t>Select peak at mouse position</t>
-  </si>
-  <si>
-    <r>
-      <t>Add p</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t>eak to s</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t>election</t>
-    </r>
-  </si>
-  <si>
-    <t>Insert new peak at mouse position</t>
+    <t>Ctrl/Cmd+N</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+O</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+S</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+Q</t>
   </si>
 </sst>
 </file>
@@ -829,11 +875,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -928,16 +972,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1272,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1287,7 +1329,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B1" s="30"/>
     </row>
@@ -1297,7 +1339,7 @@
     </row>
     <row r="3" spans="1:2" ht="20" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B3" s="5"/>
     </row>
@@ -1310,192 +1352,192 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>81</v>
+        <v>31</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>80</v>
+      <c r="A9" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" customHeight="1">
-      <c r="A10" s="26" t="s">
-        <v>182</v>
+      <c r="A10" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" customHeight="1">
       <c r="A11" s="26" t="s">
-        <v>183</v>
+        <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" customHeight="1">
       <c r="A12" s="26" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" customHeight="1">
       <c r="A13" s="26" t="s">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" customHeight="1">
       <c r="A14" s="26" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" customHeight="1">
-      <c r="A15" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>63</v>
+      <c r="A15" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17" customHeight="1">
-      <c r="A16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>105</v>
+      <c r="A16" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>8</v>
+        <v>104</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:2" ht="20" thickBot="1">
-      <c r="A22" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" ht="17" thickTop="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" ht="18">
-      <c r="A24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="28" t="s">
+    <row r="21" spans="1:2" ht="17" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:2" ht="20" thickBot="1">
+      <c r="A23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" ht="17" thickTop="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" ht="18">
+      <c r="A25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2" ht="17" customHeight="1">
-      <c r="A26" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>20</v>
-      </c>
+    <row r="26" spans="1:2">
+      <c r="A26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2" ht="17" customHeight="1">
-      <c r="A27" s="17" t="s">
-        <v>109</v>
+      <c r="A27" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="15" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="17" customHeight="1">
+      <c r="A29" s="17" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>49</v>
-      </c>
       <c r="B29" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>127</v>
@@ -1503,26 +1545,26 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="15" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="17" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="B33" s="15" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" customHeight="1">
@@ -1530,84 +1572,84 @@
         <v>115</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" customHeight="1">
       <c r="A35" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" customHeight="1">
       <c r="A36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" customHeight="1">
       <c r="A37" s="17" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>144</v>
@@ -1615,10 +1657,10 @@
     </row>
     <row r="45" spans="1:2" ht="17" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" customHeight="1">
@@ -1626,73 +1668,73 @@
         <v>149</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" customHeight="1">
       <c r="A47" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="48" spans="1:2" ht="17" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="49" spans="1:2" ht="17" customHeight="1">
-      <c r="A49" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="29"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2" ht="17" customHeight="1">
-      <c r="A50" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>84</v>
-      </c>
+      <c r="A50" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="29"/>
     </row>
     <row r="51" spans="1:2" ht="17" customHeight="1">
       <c r="A51" s="14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17" customHeight="1">
-      <c r="A52" s="10" t="s">
-        <v>83</v>
+      <c r="A52" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17" customHeight="1">
-      <c r="A53" s="14" t="s">
-        <v>68</v>
+      <c r="A53" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>88</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17" customHeight="1">
@@ -1705,68 +1747,68 @@
     </row>
     <row r="57" spans="1:2" ht="17" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="16.5" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="17" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A60" s="18"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="61" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A61" s="21" t="s">
-        <v>15</v>
-      </c>
+      <c r="A61" s="18"/>
       <c r="B61" s="8"/>
     </row>
-    <row r="62" spans="1:2" ht="17" customHeight="1">
-      <c r="A62" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>93</v>
-      </c>
+    <row r="62" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A62" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="8"/>
     </row>
     <row r="63" spans="1:2" ht="17" customHeight="1">
       <c r="A63" s="10" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17" customHeight="1">
-      <c r="A64" s="17" t="s">
-        <v>17</v>
+      <c r="A64" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" customHeight="1">
@@ -1774,166 +1816,166 @@
         <v>162</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" customHeight="1">
       <c r="A68" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" customHeight="1">
+      <c r="A69" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="17" customHeight="1">
-      <c r="A69" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="17" t="s">
-        <v>31</v>
+    </row>
+    <row r="70" spans="1:5" ht="17" customHeight="1">
+      <c r="A70" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="17" customHeight="1">
-      <c r="A71" s="18"/>
-      <c r="B71" s="8"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="17" customHeight="1">
-      <c r="A72" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="A72" s="18"/>
       <c r="B72" s="8"/>
     </row>
     <row r="73" spans="1:5" ht="17" customHeight="1">
-      <c r="A73" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
-    </row>
-    <row r="75" spans="1:5" ht="17" customHeight="1">
-      <c r="A75" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="8"/>
+      <c r="A73" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" ht="17" customHeight="1">
+      <c r="A74" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="23"/>
+      <c r="B75" s="23"/>
     </row>
     <row r="76" spans="1:5" ht="17" customHeight="1">
-      <c r="A76" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="A76" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="8"/>
     </row>
     <row r="77" spans="1:5" ht="17" customHeight="1">
       <c r="A77" s="14" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E77" s="16"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="17" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>97</v>
       </c>
+      <c r="E78" s="16"/>
     </row>
     <row r="79" spans="1:5" ht="17" customHeight="1">
       <c r="A79" s="14" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="17" customHeight="1">
       <c r="A80" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17" customHeight="1">
       <c r="A81" s="14" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="B81" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="17" customHeight="1">
+      <c r="A82" s="14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="17" customHeight="1">
-      <c r="A82" s="18"/>
-      <c r="B82" s="8"/>
+      <c r="B82" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="83" spans="1:2" ht="17" customHeight="1">
-      <c r="A83" s="25" t="s">
-        <v>47</v>
-      </c>
+      <c r="A83" s="18"/>
       <c r="B83" s="8"/>
     </row>
     <row r="84" spans="1:2" ht="17" customHeight="1">
-      <c r="A84" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="A84" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="8"/>
     </row>
     <row r="85" spans="1:2" ht="17" customHeight="1">
       <c r="A85" s="17" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17" customHeight="1">
       <c r="A86" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17" customHeight="1">
       <c r="A87" s="17" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17" customHeight="1">
       <c r="A88" s="17" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17" customHeight="1">
@@ -1941,7 +1983,7 @@
         <v>164</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>152</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17" customHeight="1">
@@ -1949,156 +1991,156 @@
         <v>165</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17" customHeight="1">
       <c r="A91" s="17" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="17" customHeight="1">
       <c r="A92" s="17" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="17" customHeight="1">
       <c r="A93" s="17" t="s">
-        <v>167</v>
+        <v>44</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="17" customHeight="1">
       <c r="A94" s="17" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>168</v>
+        <v>27</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="17" customHeight="1">
       <c r="A95" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B95" s="15" t="s">
         <v>169</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="17" customHeight="1">
       <c r="A96" s="17" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="17" customHeight="1">
-      <c r="A97" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B97" s="15"/>
+      <c r="A97" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="98" spans="1:2" ht="17" customHeight="1">
-      <c r="A98" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>56</v>
-      </c>
+      <c r="A98" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B98" s="15"/>
     </row>
     <row r="99" spans="1:2" ht="17" customHeight="1">
       <c r="A99" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17" customHeight="1">
       <c r="A100" s="17" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17" customHeight="1">
       <c r="A101" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B101" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17" customHeight="1">
       <c r="A102" s="17" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17" customHeight="1">
       <c r="A103" s="17" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17" customHeight="1">
       <c r="A104" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B104" s="15" t="s">
         <v>173</v>
-      </c>
-      <c r="B104" s="15" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17" customHeight="1">
       <c r="A105" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B105" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="B105" s="15" t="s">
+    </row>
+    <row r="106" spans="1:2" ht="17" customHeight="1">
+      <c r="A106" s="17" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="17" customHeight="1">
-      <c r="A106" s="17"/>
-      <c r="B106" s="15"/>
+      <c r="B106" s="15" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="107" spans="1:2" ht="17" customHeight="1">
-      <c r="A107" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B107" s="8"/>
+      <c r="A107" s="17"/>
+      <c r="B107" s="15"/>
     </row>
     <row r="108" spans="1:2" ht="17" customHeight="1">
-      <c r="A108" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B108" s="15" t="s">
+      <c r="A108" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B108" s="8"/>
+    </row>
+    <row r="109" spans="1:2" ht="17" customHeight="1">
+      <c r="A109" s="14" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1">
-      <c r="A109" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="B109" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17" customHeight="1">
       <c r="A110" s="20" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>181</v>
@@ -2106,14 +2148,19 @@
     </row>
     <row r="111" spans="1:2" ht="17" customHeight="1">
       <c r="A111" s="20" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="23"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="17" customHeight="1">
+      <c r="A112" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="23"/>
@@ -2138,6 +2185,9 @@
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="23"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">

</xml_diff>

<commit_message>
added ZS, ZR shortcuts for storeZoom, restoreZoom
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
   <si>
     <t>Shortcut</t>
   </si>
@@ -701,6 +701,18 @@
   </si>
   <si>
     <t>Ctrl/Cmd+Q</t>
+  </si>
+  <si>
+    <t>Store Zoom</t>
+  </si>
+  <si>
+    <t>ZS</t>
+  </si>
+  <si>
+    <t>Restore Zoom</t>
+  </si>
+  <si>
+    <t>ZR</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -2098,60 +2110,60 @@
     </row>
     <row r="104" spans="1:2" ht="17" customHeight="1">
       <c r="A104" s="17" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17" customHeight="1">
       <c r="A105" s="17" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17" customHeight="1">
       <c r="A106" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="17" customHeight="1">
+      <c r="A107" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="17" customHeight="1">
+      <c r="A108" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="17" customHeight="1">
-      <c r="A107" s="17"/>
-      <c r="B107" s="15"/>
-    </row>
-    <row r="108" spans="1:2" ht="17" customHeight="1">
-      <c r="A108" s="25" t="s">
+    <row r="109" spans="1:2" ht="17" customHeight="1">
+      <c r="A109" s="17"/>
+      <c r="B109" s="15"/>
+    </row>
+    <row r="110" spans="1:2" ht="17" customHeight="1">
+      <c r="A110" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B108" s="8"/>
-    </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1">
-      <c r="A109" s="14" t="s">
+      <c r="B110" s="8"/>
+    </row>
+    <row r="111" spans="1:2" ht="17" customHeight="1">
+      <c r="A111" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B111" s="15" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="17" customHeight="1">
-      <c r="A110" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="17" customHeight="1">
-      <c r="A111" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="17" customHeight="1">
@@ -2159,35 +2171,51 @@
         <v>48</v>
       </c>
       <c r="B112" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="17" customHeight="1">
+      <c r="A113" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1">
+      <c r="A114" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B114" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="23"/>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="23"/>
-    </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:2">
       <c r="A115" s="23"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:2">
       <c r="A116" s="23"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:2">
       <c r="A117" s="23"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:2">
       <c r="A118" s="23"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:2">
       <c r="A121" s="23"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="23"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">

</xml_diff>

<commit_message>
short labelling is now shorter
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40280" yWindow="460" windowWidth="19980" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="4820" yWindow="1100" windowWidth="20540" windowHeight="25880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="193">
   <si>
     <t>Shortcut</t>
   </si>
@@ -706,6 +701,24 @@
   </si>
   <si>
     <t>MM</t>
+  </si>
+  <si>
+    <t>Zoom in to Spectrum</t>
+  </si>
+  <si>
+    <t>Zoom out of Spectrum</t>
+  </si>
+  <si>
+    <t>ZI</t>
+  </si>
+  <si>
+    <t>ZO</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Toggle Share Y Axis Across Display</t>
   </si>
 </sst>
 </file>
@@ -1319,40 +1332,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>143</v>
       </c>
       <c r="B1" s="30"/>
     </row>
-    <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="21" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17" thickTop="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17" customHeight="1">
       <c r="A5" s="26" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1373,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17" customHeight="1">
       <c r="A6" s="26" t="s">
         <v>80</v>
       </c>
@@ -1368,7 +1381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17" customHeight="1">
       <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
@@ -1376,7 +1389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17" customHeight="1">
       <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
@@ -1384,7 +1397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17" customHeight="1">
       <c r="A9" s="26" t="s">
         <v>83</v>
       </c>
@@ -1392,7 +1405,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>84</v>
       </c>
@@ -1400,7 +1413,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="17" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1421,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="17" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>33</v>
       </c>
@@ -1416,7 +1429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="17" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1437,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="17" customHeight="1">
       <c r="A14" s="26" t="s">
         <v>13</v>
       </c>
@@ -1432,7 +1445,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="17" customHeight="1">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="17" customHeight="1">
       <c r="A16" s="27" t="s">
         <v>67</v>
       </c>
@@ -1448,7 +1461,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1456,7 +1469,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>105</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>104</v>
       </c>
@@ -1472,7 +1485,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1488,21 +1501,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="21" thickBot="1">
       <c r="A23" s="13" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="17" thickTop="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="18">
       <c r="A25" s="7" t="s">
         <v>71</v>
       </c>
@@ -1510,13 +1523,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="17" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>110</v>
       </c>
@@ -1532,7 +1545,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="17" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>112</v>
       </c>
@@ -1540,7 +1553,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
@@ -1548,7 +1561,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1569,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>123</v>
       </c>
@@ -1564,7 +1577,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>125</v>
       </c>
@@ -1572,7 +1585,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="17" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>115</v>
       </c>
@@ -1580,7 +1593,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="17" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>116</v>
       </c>
@@ -1588,7 +1601,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="17" customHeight="1">
       <c r="A36" s="17" t="s">
         <v>118</v>
       </c>
@@ -1596,7 +1609,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="17" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>120</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="17" customHeight="1">
       <c r="A38" s="17" t="s">
         <v>140</v>
       </c>
@@ -1612,7 +1625,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>138</v>
       </c>
@@ -1620,7 +1633,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="17" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
@@ -1628,7 +1641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>69</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>131</v>
       </c>
@@ -1644,7 +1657,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="17" customHeight="1">
       <c r="A43" s="17" t="s">
         <v>141</v>
       </c>
@@ -1652,7 +1665,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="17" customHeight="1">
       <c r="A44" s="17" t="s">
         <v>145</v>
       </c>
@@ -1660,7 +1673,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="17" customHeight="1">
       <c r="A45" s="17" t="s">
         <v>147</v>
       </c>
@@ -1668,7 +1681,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="17" customHeight="1">
       <c r="A46" s="17" t="s">
         <v>148</v>
       </c>
@@ -1676,7 +1689,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="17" customHeight="1">
       <c r="A47" s="17" t="s">
         <v>150</v>
       </c>
@@ -1684,7 +1697,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="17" customHeight="1">
       <c r="A48" s="17" t="s">
         <v>185</v>
       </c>
@@ -1692,507 +1705,531 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
+    <row r="49" spans="1:2" ht="17" customHeight="1">
+      <c r="A49" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" customHeight="1">
+      <c r="A50" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" customHeight="1">
+      <c r="A51" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" customHeight="1">
+      <c r="A52" s="18"/>
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="1:2" ht="17" customHeight="1">
+      <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="29"/>
-    </row>
-    <row r="51" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+      <c r="B53" s="29"/>
+    </row>
+    <row r="54" spans="1:2" ht="17" customHeight="1">
+      <c r="A54" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
+    <row r="55" spans="1:2" ht="17" customHeight="1">
+      <c r="A55" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B55" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+    <row r="56" spans="1:2" ht="17" customHeight="1">
+      <c r="A56" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B56" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+    <row r="57" spans="1:2" ht="17" customHeight="1">
+      <c r="A57" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+    <row r="58" spans="1:2" ht="17" customHeight="1">
+      <c r="A58" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
+    <row r="59" spans="1:2" ht="17" customHeight="1">
+      <c r="A59" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+    <row r="60" spans="1:2" ht="17" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
+    <row r="61" spans="1:2" ht="17" customHeight="1">
+      <c r="A61" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B61" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
+    <row r="62" spans="1:2" ht="17" customHeight="1">
+      <c r="A62" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B62" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
+    <row r="63" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A63" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B63" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="21" t="s">
+    <row r="64" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A64" s="18"/>
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A65" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:2" ht="17" customHeight="1">
+      <c r="A66" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B66" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
+    <row r="67" spans="1:2" ht="17" customHeight="1">
+      <c r="A67" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B67" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="17" t="s">
+    <row r="68" spans="1:2" ht="17" customHeight="1">
+      <c r="A68" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B68" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
+    <row r="69" spans="1:2" ht="17" customHeight="1">
+      <c r="A69" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B69" s="15" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="17" t="s">
+    <row r="70" spans="1:2" ht="17" customHeight="1">
+      <c r="A70" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B70" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
+    <row r="71" spans="1:2" ht="17" customHeight="1">
+      <c r="A71" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
+    <row r="72" spans="1:2" ht="17" customHeight="1">
+      <c r="A72" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B72" s="15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="24" t="s">
+    <row r="73" spans="1:2" ht="17" customHeight="1">
+      <c r="A73" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B73" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+    <row r="74" spans="1:2" ht="14">
+      <c r="A74" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B74" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="25" t="s">
+    <row r="75" spans="1:2" ht="17" customHeight="1">
+      <c r="A75" s="18"/>
+      <c r="B75" s="8"/>
+    </row>
+    <row r="76" spans="1:2" ht="17" customHeight="1">
+      <c r="A76" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="8"/>
-    </row>
-    <row r="74" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+      <c r="B76" s="8"/>
+    </row>
+    <row r="77" spans="1:2" ht="17" customHeight="1">
+      <c r="A77" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B77" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
-    </row>
-    <row r="76" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="25" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
+    </row>
+    <row r="79" spans="1:2" ht="17" customHeight="1">
+      <c r="A79" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B76" s="8"/>
-    </row>
-    <row r="77" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="14" t="s">
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="1:2" ht="17" customHeight="1">
+      <c r="A80" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B80" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="14" t="s">
+    <row r="81" spans="1:5" ht="17" customHeight="1">
+      <c r="A81" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B81" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E78" s="16"/>
-    </row>
-    <row r="79" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="14" t="s">
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1">
+      <c r="A82" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B82" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="14" t="s">
+    <row r="83" spans="1:5" ht="17" customHeight="1">
+      <c r="A83" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B83" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="14" t="s">
+    <row r="84" spans="1:5" ht="17" customHeight="1">
+      <c r="A84" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B84" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14" t="s">
+    <row r="85" spans="1:5" ht="17" customHeight="1">
+      <c r="A85" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B85" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="8"/>
-    </row>
-    <row r="84" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="25" t="s">
+    <row r="86" spans="1:5" ht="17" customHeight="1">
+      <c r="A86" s="18"/>
+      <c r="B86" s="8"/>
+    </row>
+    <row r="87" spans="1:5" ht="17" customHeight="1">
+      <c r="A87" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B84" s="8"/>
-    </row>
-    <row r="85" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
+      <c r="B87" s="8"/>
+    </row>
+    <row r="88" spans="1:5" ht="17" customHeight="1">
+      <c r="A88" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B88" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
+    <row r="89" spans="1:5" ht="17" customHeight="1">
+      <c r="A89" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B89" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="17" t="s">
+    <row r="90" spans="1:5" ht="17" customHeight="1">
+      <c r="A90" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B90" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="17" t="s">
+    <row r="91" spans="1:5" ht="17" customHeight="1">
+      <c r="A91" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B91" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
+    <row r="92" spans="1:5" ht="17" customHeight="1">
+      <c r="A92" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B92" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B93" s="15" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
+    <row r="94" spans="1:5" ht="17" customHeight="1">
+      <c r="A94" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B94" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
+    <row r="95" spans="1:5" ht="17" customHeight="1">
+      <c r="A95" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B95" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
+    <row r="96" spans="1:5" ht="17" customHeight="1">
+      <c r="A96" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B96" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
+    <row r="97" spans="1:2" ht="17" customHeight="1">
+      <c r="A97" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B97" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
+    <row r="98" spans="1:2" ht="17" customHeight="1">
+      <c r="A98" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B98" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17" t="s">
+    <row r="99" spans="1:2" ht="17" customHeight="1">
+      <c r="A99" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B99" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
+    <row r="100" spans="1:2" ht="17" customHeight="1">
+      <c r="A100" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B100" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="22" t="s">
+    <row r="101" spans="1:2" ht="17" customHeight="1">
+      <c r="A101" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B98" s="15"/>
-    </row>
-    <row r="99" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
+      <c r="B101" s="15"/>
+    </row>
+    <row r="102" spans="1:2" ht="17" customHeight="1">
+      <c r="A102" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B102" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="17" t="s">
+    <row r="103" spans="1:2" ht="17" customHeight="1">
+      <c r="A103" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B103" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="17" t="s">
+    <row r="104" spans="1:2" ht="17" customHeight="1">
+      <c r="A104" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B104" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
+    <row r="105" spans="1:2" ht="17" customHeight="1">
+      <c r="A105" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B105" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
+    <row r="106" spans="1:2" ht="17" customHeight="1">
+      <c r="A106" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B106" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17" t="s">
+    <row r="107" spans="1:2" ht="17" customHeight="1">
+      <c r="A107" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B107" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17" t="s">
+    <row r="108" spans="1:2" ht="17" customHeight="1">
+      <c r="A108" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
+    <row r="109" spans="1:2" ht="17" customHeight="1">
+      <c r="A109" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B109" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="17"/>
-      <c r="B107" s="15"/>
-    </row>
-    <row r="108" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="25" t="s">
+    <row r="110" spans="1:2" ht="17" customHeight="1">
+      <c r="A110" s="17"/>
+      <c r="B110" s="15"/>
+    </row>
+    <row r="111" spans="1:2" ht="17" customHeight="1">
+      <c r="A111" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B108" s="8"/>
-    </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="14" t="s">
+      <c r="B111" s="8"/>
+    </row>
+    <row r="112" spans="1:2" ht="17" customHeight="1">
+      <c r="A112" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B112" s="15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="20" t="s">
+    <row r="113" spans="1:2" ht="17" customHeight="1">
+      <c r="A113" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B113" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="20" t="s">
+    <row r="114" spans="1:2" ht="17" customHeight="1">
+      <c r="A114" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B111" s="15" t="s">
+      <c r="B114" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="20" t="s">
+    <row r="115" spans="1:2" ht="17" customHeight="1">
+      <c r="A115" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B112" s="15" t="s">
+      <c r="B115" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="23"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="23"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="23"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2">
       <c r="A116" s="23"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2">
       <c r="A117" s="23"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2">
       <c r="A118" s="23"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121" s="23"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="23"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="23"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">
@@ -2204,5 +2241,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Shortcuts to remove Blank Displays
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1100" windowWidth="20540" windowHeight="25880" tabRatio="500"/>
+    <workbookView xWindow="43840" yWindow="460" windowWidth="20540" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
   <si>
     <t>Shortcut</t>
   </si>
@@ -336,9 +341,6 @@
     <t>New project</t>
   </si>
   <si>
-    <t>New Blank Display</t>
-  </si>
-  <si>
     <t>Peak Table</t>
   </si>
   <si>
@@ -376,9 +378,6 @@
   </si>
   <si>
     <t>SA</t>
-  </si>
-  <si>
-    <t>ND</t>
   </si>
   <si>
     <t>LT</t>
@@ -1332,56 +1331,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:XFD88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" customHeight="1">
+    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="30"/>
     </row>
-    <row r="2" spans="1:2" ht="14" customHeight="1">
+    <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1">
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" ht="17" thickTop="1">
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="17" customHeight="1">
+    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" customHeight="1">
+    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" customHeight="1">
+    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
@@ -1397,31 +1396,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" customHeight="1">
+    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" customHeight="1">
+    </row>
+    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>33</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" customHeight="1">
+    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>4</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" customHeight="1">
+    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>13</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" customHeight="1">
+    <row r="15" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" customHeight="1">
+    <row r="16" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>67</v>
       </c>
@@ -1461,31 +1460,31 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" customHeight="1">
+    <row r="17" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" customHeight="1">
+    <row r="19" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" customHeight="1">
+    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1501,21 +1500,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" ht="21" thickBot="1">
+    <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" ht="17" thickTop="1">
+    <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="18">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>71</v>
       </c>
@@ -1523,13 +1522,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" ht="17" customHeight="1">
+    <row r="27" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1537,103 +1536,103 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17" customHeight="1">
+    <row r="28" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B29" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B33" s="15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="17" customHeight="1">
+    <row r="34" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" customHeight="1">
-      <c r="A35" s="17" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" customHeight="1">
-      <c r="A36" s="17" t="s">
+    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B37" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1">
-      <c r="A37" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="17" customHeight="1">
+    <row r="38" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="17" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" customHeight="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" customHeight="1">
+    <row r="41" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>69</v>
       </c>
@@ -1649,153 +1648,153 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" customHeight="1">
+    <row r="42" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" customHeight="1">
-      <c r="A44" s="17" t="s">
+    <row r="45" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" customHeight="1">
-      <c r="A45" s="17" t="s">
+    <row r="46" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="17" customHeight="1">
-      <c r="A46" s="17" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" customHeight="1">
-      <c r="A47" s="17" t="s">
+      <c r="B47" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="17" customHeight="1">
+    </row>
+    <row r="48" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="17" customHeight="1">
-      <c r="A49" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B49" s="15" t="s">
+      <c r="B50" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="15" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17" customHeight="1">
-      <c r="A50" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" customHeight="1">
-      <c r="A51" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" customHeight="1">
+    <row r="52" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
       <c r="B52" s="8"/>
     </row>
-    <row r="53" spans="1:2" ht="17" customHeight="1">
+    <row r="53" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B53" s="29"/>
     </row>
-    <row r="54" spans="1:2" ht="17" customHeight="1">
+    <row r="54" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="17" customHeight="1">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="17" customHeight="1">
-      <c r="A56" s="10" t="s">
+      <c r="B56" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="17" customHeight="1">
+    </row>
+    <row r="57" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>73</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="17" customHeight="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="17" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="17" customHeight="1">
+    </row>
+    <row r="60" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="17" customHeight="1">
+    </row>
+    <row r="61" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>74</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" customHeight="1">
+    <row r="62" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>75</v>
       </c>
@@ -1811,81 +1810,81 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5" customHeight="1">
+    <row r="63" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="16.5" customHeight="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18"/>
       <c r="B64" s="8"/>
     </row>
-    <row r="65" spans="1:2" ht="16.5" customHeight="1">
+    <row r="65" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B65" s="8"/>
     </row>
-    <row r="66" spans="1:2" ht="17" customHeight="1">
+    <row r="66" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="17" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" customHeight="1">
+    <row r="68" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="17" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="17" customHeight="1">
-      <c r="A70" s="17" t="s">
-        <v>161</v>
-      </c>
       <c r="B70" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="17" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="17" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="17" customHeight="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
         <v>25</v>
       </c>
@@ -1893,43 +1892,43 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="17" customHeight="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18"/>
       <c r="B75" s="8"/>
     </row>
-    <row r="76" spans="1:2" ht="17" customHeight="1">
+    <row r="76" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="8"/>
     </row>
-    <row r="77" spans="1:2" ht="17" customHeight="1">
+    <row r="77" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="23"/>
       <c r="B78" s="23"/>
     </row>
-    <row r="79" spans="1:2" ht="17" customHeight="1">
+    <row r="79" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25" t="s">
         <v>51</v>
       </c>
       <c r="B79" s="8"/>
     </row>
-    <row r="80" spans="1:2" ht="17" customHeight="1">
+    <row r="80" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
         <v>30</v>
       </c>
@@ -1937,32 +1936,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1">
+    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E81" s="16"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1">
-      <c r="A82" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1">
+    </row>
+    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
         <v>37</v>
       </c>
@@ -1970,151 +1969,151 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1">
+    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="18"/>
       <c r="B86" s="8"/>
     </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1">
+    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B87" s="8"/>
     </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1">
+    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1">
-      <c r="A89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1">
-      <c r="A90" s="17" t="s">
-        <v>42</v>
-      </c>
       <c r="B90" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1">
-      <c r="A93" s="17" t="s">
+      <c r="B93" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B93" s="15" t="s">
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1">
-      <c r="A94" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B94" s="15" t="s">
+      <c r="B97" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1">
-      <c r="A95" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1">
-      <c r="A96" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="17" customHeight="1">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="B97" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="17" customHeight="1">
-      <c r="A98" s="17" t="s">
-        <v>153</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="17" customHeight="1">
+    <row r="99" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="17" customHeight="1">
-      <c r="A100" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="17" customHeight="1">
-      <c r="A101" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B101" s="15"/>
-    </row>
-    <row r="102" spans="1:2" ht="17" customHeight="1">
+      <c r="B100" s="15"/>
+    </row>
+    <row r="101" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="17" customHeight="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="17" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
         <v>133</v>
       </c>
@@ -2122,23 +2121,23 @@
         <v>134</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="17" customHeight="1">
+    <row r="105" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="17" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="17" customHeight="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>170</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="17" customHeight="1">
+    <row r="108" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
         <v>172</v>
       </c>
@@ -2154,82 +2153,74 @@
         <v>173</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1">
-      <c r="A109" s="17" t="s">
+    <row r="109" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="17"/>
+      <c r="B109" s="15"/>
+    </row>
+    <row r="110" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B110" s="8"/>
+    </row>
+    <row r="111" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B111" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="17" customHeight="1">
-      <c r="A110" s="17"/>
-      <c r="B110" s="15"/>
-    </row>
-    <row r="111" spans="1:2" ht="17" customHeight="1">
-      <c r="A111" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B111" s="8"/>
-    </row>
-    <row r="112" spans="1:2" ht="17" customHeight="1">
-      <c r="A112" s="14" t="s">
-        <v>176</v>
+    <row r="112" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1">
+    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="17" customHeight="1">
-      <c r="A115" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="23"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="23"/>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">
@@ -2241,10 +2232,5 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added marks event to Gui
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43840" yWindow="460" windowWidth="20540" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="15580" yWindow="1240" windowWidth="19500" windowHeight="23300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="193">
   <si>
     <t>Shortcut</t>
   </si>
@@ -301,12 +296,6 @@
     <t>Show/Hide Toolbar</t>
   </si>
   <si>
-    <t>Reset Zoom</t>
-  </si>
-  <si>
-    <t>RZ</t>
-  </si>
-  <si>
     <t>Move single peak</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -718,6 +707,18 @@
   </si>
   <si>
     <t>Toggle Share Y Axis Across Display</t>
+  </si>
+  <si>
+    <t>ZR</t>
+  </si>
+  <si>
+    <t>Store Zoom</t>
+  </si>
+  <si>
+    <t>ZS</t>
+  </si>
+  <si>
+    <t>Restore Zoom</t>
   </si>
 </sst>
 </file>
@@ -892,9 +893,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -989,14 +992,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1331,56 +1336,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="30"/>
     </row>
-    <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="21" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17" thickTop="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17" customHeight="1">
       <c r="A5" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17" customHeight="1">
       <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
@@ -1388,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17" customHeight="1">
       <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
@@ -1396,31 +1401,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17" customHeight="1">
       <c r="A9" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" customHeight="1">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" ht="17" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>33</v>
       </c>
@@ -1428,7 +1433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="17" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="17" customHeight="1">
       <c r="A14" s="26" t="s">
         <v>13</v>
       </c>
@@ -1444,7 +1449,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="17" customHeight="1">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
@@ -1452,39 +1457,39 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="17" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1492,7 +1497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1500,35 +1505,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="21" thickBot="1">
       <c r="A23" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="17" thickTop="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="18">
       <c r="A25" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="17" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1536,103 +1541,103 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" customHeight="1">
+      <c r="A29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B29" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B33" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="17" customHeight="1">
       <c r="A34" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="17" customHeight="1">
+      <c r="A36" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+    <row r="37" spans="1:2" ht="17" customHeight="1">
+      <c r="A37" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B37" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="17" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
@@ -1640,251 +1645,251 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17" customHeight="1">
+      <c r="A44" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+    <row r="45" spans="1:2" ht="17" customHeight="1">
+      <c r="A45" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="46" spans="1:2" ht="17" customHeight="1">
+      <c r="A46" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="17" customHeight="1">
+      <c r="A47" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="B47" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:2" ht="17" customHeight="1">
       <c r="A48" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17" customHeight="1">
+      <c r="A49" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" customHeight="1">
+      <c r="A50" s="17" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="15" t="s">
+      <c r="B50" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" customHeight="1">
+      <c r="A51" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="17" customHeight="1">
       <c r="A52" s="18"/>
       <c r="B52" s="8"/>
     </row>
-    <row r="53" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="17" customHeight="1">
       <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B53" s="29"/>
     </row>
-    <row r="54" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="17" customHeight="1">
       <c r="A54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" customHeight="1">
+      <c r="A55" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" customHeight="1">
+      <c r="A56" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="17" customHeight="1">
+      <c r="A57" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="17" customHeight="1">
+      <c r="A58" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="B58" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:2" ht="17" customHeight="1">
       <c r="A59" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:2" ht="17" customHeight="1">
       <c r="A60" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:2" ht="17" customHeight="1">
       <c r="A61" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="17" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="16.5" customHeight="1">
       <c r="A63" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16.5" customHeight="1">
       <c r="A64" s="18"/>
       <c r="B64" s="8"/>
     </row>
-    <row r="65" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="16.5" customHeight="1">
       <c r="A65" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B65" s="8"/>
     </row>
-    <row r="66" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="17" customHeight="1">
       <c r="A66" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="17" customHeight="1">
       <c r="A67" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="17" customHeight="1">
       <c r="A68" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="17" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17" customHeight="1">
+      <c r="A70" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>159</v>
-      </c>
       <c r="B70" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="17" customHeight="1">
       <c r="A71" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="17" customHeight="1">
       <c r="A72" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="17" customHeight="1">
       <c r="A73" s="24" t="s">
         <v>25</v>
       </c>
@@ -1892,43 +1897,43 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="14">
       <c r="A74" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="17" customHeight="1">
       <c r="A75" s="18"/>
       <c r="B75" s="8"/>
     </row>
-    <row r="76" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="17" customHeight="1">
       <c r="A76" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="8"/>
     </row>
-    <row r="77" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="17" customHeight="1">
       <c r="A77" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="23"/>
       <c r="B78" s="23"/>
     </row>
-    <row r="79" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="17" customHeight="1">
       <c r="A79" s="25" t="s">
         <v>51</v>
       </c>
       <c r="B79" s="8"/>
     </row>
-    <row r="80" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="17" customHeight="1">
       <c r="A80" s="14" t="s">
         <v>30</v>
       </c>
@@ -1936,32 +1941,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="17" customHeight="1">
       <c r="A81" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1">
+      <c r="A82" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B82" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E81" s="16"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" ht="17" customHeight="1">
       <c r="A83" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" customHeight="1">
       <c r="A84" s="14" t="s">
         <v>37</v>
       </c>
@@ -1969,25 +1974,25 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="17" customHeight="1">
       <c r="A85" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" customHeight="1">
       <c r="A86" s="18"/>
       <c r="B86" s="8"/>
     </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="17" customHeight="1">
       <c r="A87" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B87" s="8"/>
     </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="17" customHeight="1">
       <c r="A88" s="17" t="s">
         <v>41</v>
       </c>
@@ -1995,7 +2000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="17" customHeight="1">
       <c r="A89" s="17" t="s">
         <v>42</v>
       </c>
@@ -2003,39 +2008,39 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="17" customHeight="1">
       <c r="A90" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" customHeight="1">
       <c r="A91" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="17" customHeight="1">
       <c r="A92" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1">
       <c r="A94" s="17" t="s">
         <v>47</v>
       </c>
@@ -2043,53 +2048,53 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="17" customHeight="1">
       <c r="A95" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" customHeight="1">
       <c r="A96" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="17" customHeight="1">
       <c r="A97" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B97" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="17" customHeight="1">
+      <c r="A98" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="17" customHeight="1">
       <c r="A99" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="17" customHeight="1">
       <c r="A100" s="22" t="s">
         <v>63</v>
       </c>
       <c r="B100" s="15"/>
     </row>
-    <row r="101" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="17" customHeight="1">
       <c r="A101" s="17" t="s">
         <v>64</v>
       </c>
@@ -2097,97 +2102,97 @@
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" ht="17" customHeight="1">
       <c r="A102" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="17" customHeight="1">
       <c r="A103" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="17" customHeight="1">
+      <c r="A104" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B104" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B104" s="15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" ht="17" customHeight="1">
       <c r="A105" s="17" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="17" customHeight="1">
       <c r="A106" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="17" customHeight="1">
+      <c r="A107" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="17" customHeight="1">
+      <c r="A108" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="17" t="s">
+    <row r="109" spans="1:2" ht="17" customHeight="1">
+      <c r="A109" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B109" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
+    <row r="110" spans="1:2" ht="17" customHeight="1">
+      <c r="A110" s="17"/>
+      <c r="B110" s="15"/>
+    </row>
+    <row r="111" spans="1:2" ht="17" customHeight="1">
+      <c r="A111" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B111" s="8"/>
+    </row>
+    <row r="112" spans="1:2" ht="17" customHeight="1">
+      <c r="A112" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B112" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17"/>
-      <c r="B109" s="15"/>
-    </row>
-    <row r="110" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B110" s="8"/>
-    </row>
-    <row r="111" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="17" customHeight="1">
       <c r="A113" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1">
       <c r="A114" s="20" t="s">
         <v>48</v>
       </c>
@@ -2195,32 +2200,40 @@
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="23"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" ht="17" customHeight="1">
+      <c r="A115" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" s="23"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2">
       <c r="A117" s="23"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2">
       <c r="A118" s="23"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121" s="23"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2">
       <c r="A122" s="23"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2">
       <c r="A123" s="23"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">
@@ -2232,5 +2245,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stopped creation of duplicate marks - delta-position<1e-6
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45380" yWindow="460" windowWidth="19500" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="213">
   <si>
     <t>Shortcut</t>
   </si>
@@ -521,31 +516,7 @@
     <t>Ctrl/Cmd+A</t>
   </si>
   <si>
-    <r>
-      <t>Analysis V3</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t>beta2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="26"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t xml:space="preserve"> shortcuts</t>
-    </r>
-  </si>
-  <si>
     <t>PV</t>
-  </si>
-  <si>
-    <t>Toggle Phasing Pivot</t>
   </si>
   <si>
     <t>I1</t>
@@ -725,6 +696,98 @@
   <si>
     <t>Double Backspace</t>
   </si>
+  <si>
+    <t>Related</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="26"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t>Analysis V3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t>beta2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="26"/>
+        <color indexed="8"/>
+        <rFont val="Lucida Grande"/>
+      </rPr>
+      <t xml:space="preserve"> shortcuts</t>
+    </r>
+  </si>
+  <si>
+    <t>TV, TU, TD</t>
+  </si>
+  <si>
+    <t>PC, PT, TR</t>
+  </si>
+  <si>
+    <t>PC, PV, PT</t>
+  </si>
+  <si>
+    <t>XZ, YZ</t>
+  </si>
+  <si>
+    <t>XY, YZ</t>
+  </si>
+  <si>
+    <t>ZI, ZO, ZR</t>
+  </si>
+  <si>
+    <t>ZI, ZO, ZS</t>
+  </si>
+  <si>
+    <t>ZO, ZS, ZR</t>
+  </si>
+  <si>
+    <t>ZI, ZS, ZR</t>
+  </si>
+  <si>
+    <t>PC, PV, TR</t>
+  </si>
+  <si>
+    <t>PV, PT, TR</t>
+  </si>
+  <si>
+    <t>XY, XZ</t>
+  </si>
+  <si>
+    <t>TH, TU, TD</t>
+  </si>
+  <si>
+    <t>TH, TV, TD</t>
+  </si>
+  <si>
+    <t>TH, TV, TU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH, TA, PC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS, TA, PC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS, CH, PC </t>
+  </si>
+  <si>
+    <t>Set Phasing Pivot to cursor position</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
 </sst>
 </file>
 
@@ -733,7 +796,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -831,13 +894,6 @@
       <name val="Lucida Grande"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Lucida Grande"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color indexed="8"/>
@@ -862,13 +918,32 @@
       <name val="Lucida Grande"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Lucida Grande"/>
     </font>
     <font>
+      <b/>
+      <sz val="26"/>
+      <color indexed="8"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
     </font>
   </fonts>
@@ -898,7 +973,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -909,8 +984,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -968,16 +1073,13 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -987,26 +1089,62 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="40">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1343,78 +1481,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="30"/>
-    </row>
-    <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:3" ht="14" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="20" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="17" thickTop="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:3" ht="17" customHeight="1">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:3" ht="17" customHeight="1">
+      <c r="A6" s="25" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:3" ht="17" customHeight="1">
+      <c r="A7" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:3" ht="17" customHeight="1">
+      <c r="A8" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:3" ht="17" customHeight="1">
+      <c r="A9" s="25" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>81</v>
       </c>
@@ -1422,55 +1564,55 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:3" ht="17" customHeight="1">
+      <c r="A11" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:3" ht="17" customHeight="1">
+      <c r="A12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:3" ht="17" customHeight="1">
+      <c r="A13" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:3" ht="17" customHeight="1">
+      <c r="A14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:3" ht="17" customHeight="1">
+      <c r="A15" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:3" ht="17" customHeight="1">
+      <c r="A16" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1620,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>101</v>
       </c>
@@ -1486,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>100</v>
       </c>
@@ -1494,7 +1636,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1502,7 +1644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1510,35 +1652,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="20" thickBot="1">
       <c r="A23" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="17" thickTop="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="17" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1546,103 +1692,139 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>106</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>108</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>119</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>121</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>111</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" customHeight="1">
       <c r="A36" s="17" t="s">
         <v>114</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>116</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" customHeight="1">
       <c r="A38" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
@@ -1650,23 +1832,29 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>127</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" customHeight="1">
       <c r="A43" s="17" t="s">
         <v>135</v>
       </c>
@@ -1674,97 +1862,115 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="17" customHeight="1">
       <c r="A44" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" customHeight="1">
+      <c r="A45" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="46" spans="1:3" ht="17" customHeight="1">
+      <c r="A46" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+      <c r="C46" s="31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" customHeight="1">
+      <c r="A47" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="B47" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" customHeight="1">
       <c r="A48" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" customHeight="1">
+      <c r="A49" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" customHeight="1">
+      <c r="A50" s="17" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B49" s="15" t="s">
+      <c r="B50" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" customHeight="1">
+      <c r="A51" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="15" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" customHeight="1">
       <c r="A52" s="18"/>
       <c r="B52" s="8"/>
     </row>
-    <row r="53" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="17" customHeight="1">
       <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="29"/>
-    </row>
-    <row r="54" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="28"/>
+    </row>
+    <row r="54" spans="1:3" ht="17" customHeight="1">
       <c r="A54" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" customHeight="1">
       <c r="A55" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" customHeight="1">
       <c r="A56" s="10" t="s">
         <v>85</v>
       </c>
@@ -1772,15 +1978,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="17" customHeight="1">
       <c r="A57" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" customHeight="1">
       <c r="A58" s="14" t="s">
         <v>76</v>
       </c>
@@ -1788,23 +1994,23 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="17" customHeight="1">
       <c r="A59" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:3" ht="17" customHeight="1">
       <c r="A60" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:3" ht="17" customHeight="1">
       <c r="A61" s="14" t="s">
         <v>72</v>
       </c>
@@ -1812,7 +2018,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="17" customHeight="1">
       <c r="A62" s="14" t="s">
         <v>73</v>
       </c>
@@ -1820,41 +2026,47 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="16.5" customHeight="1">
       <c r="A63" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16.5" customHeight="1">
       <c r="A64" s="18"/>
       <c r="B64" s="8"/>
     </row>
-    <row r="65" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="16.5" customHeight="1">
       <c r="A65" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B65" s="8"/>
     </row>
-    <row r="66" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="17" customHeight="1">
       <c r="A66" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="15" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" customHeight="1">
       <c r="A67" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" customHeight="1">
       <c r="A68" s="17" t="s">
         <v>20</v>
       </c>
@@ -1862,47 +2074,59 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="17" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" customHeight="1">
+      <c r="A70" s="17" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>155</v>
       </c>
       <c r="B70" s="15" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" customHeight="1">
       <c r="A71" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17" customHeight="1">
       <c r="A72" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B72" s="15" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="24" t="s">
+      <c r="C72" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17" customHeight="1">
+      <c r="A73" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74" s="17" t="s">
         <v>36</v>
       </c>
@@ -1910,17 +2134,17 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="17" customHeight="1">
       <c r="A75" s="18"/>
       <c r="B75" s="8"/>
     </row>
-    <row r="76" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="25" t="s">
+    <row r="76" spans="1:3" ht="17" customHeight="1">
+      <c r="A76" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="8"/>
     </row>
-    <row r="77" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="17" customHeight="1">
       <c r="A77" s="17" t="s">
         <v>28</v>
       </c>
@@ -1928,17 +2152,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" s="23"/>
       <c r="B78" s="23"/>
     </row>
-    <row r="79" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="25" t="s">
+    <row r="79" spans="1:3" ht="17" customHeight="1">
+      <c r="A79" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B79" s="8"/>
     </row>
-    <row r="80" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="17" customHeight="1">
       <c r="A80" s="14" t="s">
         <v>30</v>
       </c>
@@ -1946,7 +2170,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="17" customHeight="1">
       <c r="A81" s="14" t="s">
         <v>92</v>
       </c>
@@ -1955,7 +2179,7 @@
       </c>
       <c r="E81" s="16"/>
     </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="17" customHeight="1">
       <c r="A82" s="14" t="s">
         <v>95</v>
       </c>
@@ -1963,7 +2187,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="17" customHeight="1">
       <c r="A83" s="14" t="s">
         <v>29</v>
       </c>
@@ -1971,7 +2195,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="17" customHeight="1">
       <c r="A84" s="14" t="s">
         <v>37</v>
       </c>
@@ -1979,7 +2203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="17" customHeight="1">
       <c r="A85" s="14" t="s">
         <v>96</v>
       </c>
@@ -1987,17 +2211,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="17" customHeight="1">
       <c r="A86" s="18"/>
       <c r="B86" s="8"/>
     </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="25" t="s">
+    <row r="87" spans="1:5" ht="17" customHeight="1">
+      <c r="A87" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B87" s="8"/>
     </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="17" customHeight="1">
       <c r="A88" s="17" t="s">
         <v>41</v>
       </c>
@@ -2005,7 +2229,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="17" customHeight="1">
       <c r="A89" s="17" t="s">
         <v>42</v>
       </c>
@@ -2013,7 +2237,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="17" customHeight="1">
       <c r="A90" s="17" t="s">
         <v>75</v>
       </c>
@@ -2021,31 +2245,31 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="17" customHeight="1">
       <c r="A91" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="17" customHeight="1">
       <c r="A92" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1">
       <c r="A94" s="17" t="s">
         <v>47</v>
       </c>
@@ -2053,7 +2277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="17" customHeight="1">
       <c r="A95" s="17" t="s">
         <v>44</v>
       </c>
@@ -2061,31 +2285,31 @@
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="17" customHeight="1">
       <c r="A96" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="17" customHeight="1">
       <c r="A97" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B97" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" customHeight="1">
+      <c r="A98" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B98" s="15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="17" customHeight="1">
       <c r="A99" s="17" t="s">
         <v>45</v>
       </c>
@@ -2093,13 +2317,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="17" customHeight="1">
       <c r="A100" s="22" t="s">
         <v>63</v>
       </c>
       <c r="B100" s="15"/>
     </row>
-    <row r="101" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="17" customHeight="1">
       <c r="A101" s="17" t="s">
         <v>64</v>
       </c>
@@ -2107,137 +2331,155 @@
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="17" customHeight="1">
       <c r="A102" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C102" s="31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" customHeight="1">
       <c r="A103" s="17" t="s">
         <v>129</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" customHeight="1">
       <c r="A104" s="17" t="s">
         <v>130</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17" customHeight="1">
       <c r="A105" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C105" s="31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17" customHeight="1">
+      <c r="A106" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
-        <v>190</v>
-      </c>
       <c r="B106" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+      <c r="C106" s="31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17" customHeight="1">
       <c r="A107" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C107" s="31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" customHeight="1">
+      <c r="A108" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
+      <c r="C108" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17" customHeight="1">
+      <c r="A109" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B109" s="15" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" customHeight="1">
       <c r="A110" s="17"/>
       <c r="B110" s="15"/>
     </row>
-    <row r="111" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="25" t="s">
+    <row r="111" spans="1:3" ht="17" customHeight="1">
+      <c r="A111" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B111" s="8"/>
     </row>
-    <row r="112" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="17" customHeight="1">
       <c r="A112" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="17" customHeight="1">
       <c r="A113" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1">
       <c r="A114" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="17" customHeight="1">
       <c r="A115" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" s="23"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2">
       <c r="A117" s="23"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2">
       <c r="A118" s="23"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121" s="23"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2">
       <c r="A122" s="23"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2">
       <c r="A123" s="23"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2">
       <c r="A124" s="23"/>
     </row>
   </sheetData>
@@ -2245,10 +2487,15 @@
     <sortCondition ref="A6:A21"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed overloaded 'cs' for screen
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39240" yWindow="460" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="219">
   <si>
     <t>Shortcut</t>
   </si>
@@ -798,6 +793,18 @@
   </si>
   <si>
     <t>TabTab</t>
+  </si>
+  <si>
+    <t>Cycle Peak Labelling</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Cycle Peak Symbols</t>
   </si>
 </sst>
 </file>
@@ -984,9 +991,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="40">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1116,7 +1127,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="40">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1136,6 +1147,8 @@
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1156,6 +1169,8 @@
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1490,13 +1505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
@@ -1505,29 +1520,29 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>190</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" thickTop="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
@@ -1535,7 +1550,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>77</v>
       </c>
@@ -1543,7 +1558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" customHeight="1">
       <c r="A7" s="25" t="s">
         <v>22</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>31</v>
       </c>
@@ -1559,7 +1574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17" customHeight="1">
       <c r="A9" s="25" t="s">
         <v>80</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>81</v>
       </c>
@@ -1575,7 +1590,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17" customHeight="1">
       <c r="A11" s="25" t="s">
         <v>2</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17" customHeight="1">
       <c r="A12" s="25" t="s">
         <v>33</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17" customHeight="1">
       <c r="A13" s="25" t="s">
         <v>4</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17" customHeight="1">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17" customHeight="1">
       <c r="A15" s="25" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1630,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" customHeight="1">
       <c r="A16" s="26" t="s">
         <v>65</v>
       </c>
@@ -1623,7 +1638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1631,7 +1646,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>101</v>
       </c>
@@ -1639,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>100</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1655,7 +1670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1663,22 +1678,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="21" thickBot="1">
       <c r="A23" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17" thickTop="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="7" t="s">
         <v>69</v>
       </c>
@@ -1689,13 +1704,13 @@
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="17" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1703,7 +1718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>106</v>
       </c>
@@ -1714,7 +1729,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="17" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>108</v>
       </c>
@@ -1725,7 +1740,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
@@ -1736,7 +1751,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
@@ -1747,7 +1762,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>119</v>
       </c>
@@ -1758,7 +1773,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>121</v>
       </c>
@@ -1769,7 +1784,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="17" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>111</v>
       </c>
@@ -1780,7 +1795,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="17" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>112</v>
       </c>
@@ -1791,7 +1806,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="17" customHeight="1">
       <c r="A36" s="17" t="s">
         <v>114</v>
       </c>
@@ -1802,7 +1817,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="17" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>116</v>
       </c>
@@ -1813,7 +1828,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="17" customHeight="1">
       <c r="A38" s="17" t="s">
         <v>134</v>
       </c>
@@ -1824,7 +1839,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>132</v>
       </c>
@@ -1835,7 +1850,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="17" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
@@ -1843,7 +1858,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>67</v>
       </c>
@@ -1854,7 +1869,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>127</v>
       </c>
@@ -1865,7 +1880,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="17" customHeight="1">
       <c r="A43" s="17" t="s">
         <v>135</v>
       </c>
@@ -1873,7 +1888,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="17" customHeight="1">
       <c r="A44" s="17" t="s">
         <v>209</v>
       </c>
@@ -1884,7 +1899,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="17" customHeight="1">
       <c r="A45" s="17" t="s">
         <v>139</v>
       </c>
@@ -1892,7 +1907,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="17" customHeight="1">
       <c r="A46" s="17" t="s">
         <v>140</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="17" customHeight="1">
       <c r="A47" s="17" t="s">
         <v>142</v>
       </c>
@@ -1914,7 +1929,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="17" customHeight="1">
       <c r="A48" s="17" t="s">
         <v>177</v>
       </c>
@@ -1922,7 +1937,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="17" customHeight="1">
       <c r="A49" s="17" t="s">
         <v>179</v>
       </c>
@@ -1933,7 +1948,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="17" customHeight="1">
       <c r="A50" s="17" t="s">
         <v>180</v>
       </c>
@@ -1944,7 +1959,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="17" customHeight="1">
       <c r="A51" s="17" t="s">
         <v>184</v>
       </c>
@@ -1955,554 +1970,576 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
+    <row r="52" spans="1:3" ht="17" customHeight="1">
+      <c r="A52" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" customHeight="1">
+      <c r="A53" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" customHeight="1">
+      <c r="A54" s="18"/>
+      <c r="B54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" ht="17" customHeight="1">
+      <c r="A55" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="28"/>
-    </row>
-    <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+      <c r="B55" s="28"/>
+    </row>
+    <row r="56" spans="1:3" ht="17" customHeight="1">
+      <c r="A56" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B56" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+    <row r="57" spans="1:3" ht="17" customHeight="1">
+      <c r="A57" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+    <row r="58" spans="1:3" ht="17" customHeight="1">
+      <c r="A58" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+    <row r="59" spans="1:3" ht="17" customHeight="1">
+      <c r="A59" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
+    <row r="60" spans="1:3" ht="17" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
+    <row r="61" spans="1:3" ht="17" customHeight="1">
+      <c r="A61" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B61" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
+    <row r="62" spans="1:3" ht="17" customHeight="1">
+      <c r="A62" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B62" s="15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
+    <row r="63" spans="1:3" ht="17" customHeight="1">
+      <c r="A63" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B63" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
+    <row r="64" spans="1:3" ht="17" customHeight="1">
+      <c r="A64" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B64" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
+    <row r="65" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A65" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="21" t="s">
+    <row r="66" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A66" s="18"/>
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A67" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="8"/>
-    </row>
-    <row r="66" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" ht="17" customHeight="1">
+      <c r="A68" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B68" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C66" s="29" t="s">
+      <c r="C68" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
+    <row r="69" spans="1:3" ht="17" customHeight="1">
+      <c r="A69" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B69" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C69" s="29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
+    <row r="70" spans="1:3" ht="17" customHeight="1">
+      <c r="A70" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B70" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
+    <row r="71" spans="1:3" ht="17" customHeight="1">
+      <c r="A71" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C71" s="29" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
+    <row r="72" spans="1:3" ht="17" customHeight="1">
+      <c r="A72" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B72" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C72" s="29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+    <row r="73" spans="1:3" ht="17" customHeight="1">
+      <c r="A73" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B73" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="29" t="s">
+      <c r="C73" s="29" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
+    <row r="74" spans="1:3" ht="17" customHeight="1">
+      <c r="A74" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B74" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C72" s="29" t="s">
+      <c r="C74" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
+    <row r="75" spans="1:3" ht="17" customHeight="1">
+      <c r="A75" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B75" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+    <row r="76" spans="1:3" ht="14">
+      <c r="A76" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B76" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="8"/>
-    </row>
-    <row r="76" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24" t="s">
+    <row r="77" spans="1:3" ht="17" customHeight="1">
+      <c r="A77" s="18"/>
+      <c r="B77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" ht="17" customHeight="1">
+      <c r="A78" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="8"/>
-    </row>
-    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
+      <c r="B78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" ht="17" customHeight="1">
+      <c r="A79" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B79" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="23"/>
-      <c r="B78" s="23"/>
-    </row>
-    <row r="79" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="24" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
+    </row>
+    <row r="81" spans="1:5" ht="17" customHeight="1">
+      <c r="A81" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B79" s="8"/>
-    </row>
-    <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="14" t="s">
+      <c r="B81" s="8"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1">
+      <c r="A82" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B82" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="14" t="s">
+    <row r="83" spans="1:5" ht="17" customHeight="1">
+      <c r="A83" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B83" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E81" s="16"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14" t="s">
+      <c r="E83" s="16"/>
+    </row>
+    <row r="84" spans="1:5" ht="17" customHeight="1">
+      <c r="A84" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B84" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="14" t="s">
+    <row r="85" spans="1:5" ht="17" customHeight="1">
+      <c r="A85" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B85" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="14" t="s">
+    <row r="86" spans="1:5" ht="17" customHeight="1">
+      <c r="A86" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B86" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="14" t="s">
+    <row r="87" spans="1:5" ht="17" customHeight="1">
+      <c r="A87" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B87" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="8"/>
-    </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24" t="s">
+    <row r="88" spans="1:5" ht="17" customHeight="1">
+      <c r="A88" s="18"/>
+      <c r="B88" s="8"/>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1">
+      <c r="A89" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B87" s="8"/>
-    </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="17" t="s">
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" spans="1:5" ht="17" customHeight="1">
+      <c r="A90" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B90" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
+    <row r="91" spans="1:5" ht="17" customHeight="1">
+      <c r="A91" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B91" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
+    <row r="92" spans="1:5" ht="17" customHeight="1">
+      <c r="A92" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B92" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B93" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
+    <row r="94" spans="1:5" ht="17" customHeight="1">
+      <c r="A94" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B94" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
+    <row r="95" spans="1:5" ht="17" customHeight="1">
+      <c r="A95" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B95" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
+    <row r="96" spans="1:5" ht="17" customHeight="1">
+      <c r="A96" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B96" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
+    <row r="97" spans="1:3" ht="17" customHeight="1">
+      <c r="A97" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B97" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17" t="s">
+    <row r="98" spans="1:3" ht="17" customHeight="1">
+      <c r="A98" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B98" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
+    <row r="99" spans="1:3" ht="17" customHeight="1">
+      <c r="A99" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B99" s="15" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
+    <row r="100" spans="1:3" ht="17" customHeight="1">
+      <c r="A100" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B100" s="15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
+    <row r="101" spans="1:3" ht="17" customHeight="1">
+      <c r="A101" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B101" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="22" t="s">
+    <row r="102" spans="1:3" ht="17" customHeight="1">
+      <c r="A102" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B100" s="15"/>
-    </row>
-    <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="17" t="s">
+      <c r="B102" s="15"/>
+    </row>
+    <row r="103" spans="1:3" ht="17" customHeight="1">
+      <c r="A103" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B103" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
+    <row r="104" spans="1:3" ht="17" customHeight="1">
+      <c r="A104" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B104" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C102" s="29" t="s">
+      <c r="C104" s="29" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
+    <row r="105" spans="1:3" ht="17" customHeight="1">
+      <c r="A105" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B105" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C103" s="15"/>
-    </row>
-    <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17" t="s">
+      <c r="C105" s="15"/>
+    </row>
+    <row r="106" spans="1:3" ht="17" customHeight="1">
+      <c r="A106" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B106" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="C104" s="15"/>
-    </row>
-    <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17" t="s">
+      <c r="C106" s="15"/>
+    </row>
+    <row r="107" spans="1:3" ht="17" customHeight="1">
+      <c r="A107" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B107" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C105" s="15"/>
-    </row>
-    <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
+      <c r="C107" s="15"/>
+    </row>
+    <row r="108" spans="1:3" ht="17" customHeight="1">
+      <c r="A108" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C106" s="29" t="s">
+      <c r="C108" s="29" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="17" t="s">
+    <row r="109" spans="1:3" ht="17" customHeight="1">
+      <c r="A109" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B109" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C107" s="29" t="s">
+      <c r="C109" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
+    <row r="110" spans="1:3" ht="17" customHeight="1">
+      <c r="A110" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B110" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C108" s="29" t="s">
+      <c r="C110" s="29" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
+    <row r="111" spans="1:3" ht="17" customHeight="1">
+      <c r="A111" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B111" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C109" s="29" t="s">
+      <c r="C111" s="29" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="17" t="s">
+    <row r="112" spans="1:3" ht="17" customHeight="1">
+      <c r="A112" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B112" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C110" s="29" t="s">
+      <c r="C112" s="29" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="17"/>
-      <c r="B111" s="15"/>
-    </row>
-    <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="24" t="s">
+    <row r="113" spans="1:2" ht="17" customHeight="1">
+      <c r="A113" s="17"/>
+      <c r="B113" s="15"/>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1">
+      <c r="A114" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B112" s="8"/>
-    </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="14" t="s">
+      <c r="B114" s="8"/>
+    </row>
+    <row r="115" spans="1:2" ht="17" customHeight="1">
+      <c r="A115" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B113" s="15" t="s">
+      <c r="B115" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" ht="17" customHeight="1">
       <c r="A116" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B116" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="17" customHeight="1">
+      <c r="A117" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="17" customHeight="1">
+      <c r="A118" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B118" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="23"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="23"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119" s="23"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121" s="23"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2">
       <c r="A122" s="23"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2">
       <c r="A123" s="23"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2">
       <c r="A124" s="23"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2">
       <c r="A125" s="23"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="23"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">
@@ -2514,5 +2551,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
strip headers can be closed with right mouse menu changed shortcut for printing to cmd+P added preferences shortcut to cmd+,
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/AnalysisV3/doc/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F17B4F-03D5-2A45-98C3-1B8DE106E349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38380" yWindow="4280" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="5340" yWindow="1520" windowWidth="25600" windowHeight="15520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="219">
   <si>
     <t>Shortcut</t>
   </si>
@@ -203,10 +204,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Ctrl/Cmd+Z</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Ctrl/Cmd+Y</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -480,9 +477,6 @@
   </si>
   <si>
     <t>PC</t>
-  </si>
-  <si>
-    <t>PR</t>
   </si>
   <si>
     <t xml:space="preserve">Snap to Extremum Current Selected Peaks </t>
@@ -681,35 +675,6 @@
     <t>Related</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="26"/>
-        <color indexed="8"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t>Analysis V3</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t>beta2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="26"/>
-        <color indexed="8"/>
-        <rFont val="Lucida Grande"/>
-      </rPr>
-      <t xml:space="preserve"> shortcuts</t>
-    </r>
-  </si>
-  <si>
     <t>TV, TU, TD</t>
   </si>
   <si>
@@ -804,16 +769,31 @@
   </si>
   <si>
     <t>Space-Space</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+Z</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+P</t>
+  </si>
+  <si>
+    <t>Analysis V3 shortcuts</t>
+  </si>
+  <si>
+    <t>Preferences</t>
+  </si>
+  <si>
+    <t>Ctrl/Cmd+,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -947,18 +927,6 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Lucida Grande"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Lucida Grande"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
@@ -1116,13 +1084,13 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1177,6 +1145,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1503,11 +1474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E126"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1520,11 +1491,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="A1" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1532,7 +1503,7 @@
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1546,12 +1517,12 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -1575,18 +1546,18 @@
     </row>
     <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1594,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1610,7 +1581,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1618,7 +1589,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1626,15 +1597,15 @@
         <v>5</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1642,12 +1613,12 @@
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -1655,10 +1626,10 @@
     </row>
     <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1683,7 +1654,7 @@
     </row>
     <row r="23" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1694,18 +1665,18 @@
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="8"/>
     </row>
@@ -1719,276 +1690,276 @@
     </row>
     <row r="28" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>105</v>
-      </c>
       <c r="C28" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>107</v>
-      </c>
       <c r="C29" s="29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="C32" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="C33" s="15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="C35" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="C36" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="C37" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>67</v>
-      </c>
       <c r="C41" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>142</v>
-      </c>
       <c r="C47" s="29" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2003,155 +1974,152 @@
     </row>
     <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>34</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="8"/>
+      <c r="B66" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="67" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="18"/>
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>19</v>
-      </c>
+      <c r="B68" s="8"/>
     </row>
     <row r="69" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C69" s="29" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>20</v>
+      <c r="A70" s="10" t="s">
+        <v>145</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>116</v>
+        <v>19</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="C73" s="29" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2162,237 +2130,239 @@
         <v>129</v>
       </c>
       <c r="C74" s="29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B76" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="8"/>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="78" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
+      <c r="A78" s="18"/>
+      <c r="B78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B78" s="8"/>
-    </row>
-    <row r="79" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
-    </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="B82" s="8"/>
     </row>
     <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="16"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>92</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E84" s="16"/>
     </row>
     <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B87" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
-      <c r="B88" s="8"/>
     </row>
     <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="24" t="s">
-        <v>51</v>
-      </c>
+      <c r="A89" s="18"/>
       <c r="B89" s="8"/>
     </row>
     <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>40</v>
-      </c>
+      <c r="A90" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>141</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>216</v>
+        <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B101" s="15"/>
+      <c r="A101" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="A102" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102" s="15"/>
     </row>
     <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C103" s="29" t="s">
-        <v>195</v>
+        <v>59</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="C104" s="15"/>
+        <v>122</v>
+      </c>
+      <c r="C104" s="29" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>205</v>
@@ -2401,41 +2371,39 @@
     </row>
     <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C106" s="15"/>
     </row>
     <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C107" s="29" t="s">
-        <v>190</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C107" s="15"/>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>179</v>
       </c>
       <c r="C108" s="29" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="C109" s="29" t="s">
         <v>188</v>
@@ -2443,70 +2411,78 @@
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C111" s="29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C112" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="17"/>
+      <c r="B113" s="15"/>
+    </row>
+    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B114" s="8"/>
+    </row>
+    <row r="115" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B111" s="15" t="s">
+      <c r="B115" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="C111" s="29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="17"/>
-      <c r="B112" s="15"/>
-    </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B113" s="8"/>
-    </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="23"/>
+    <row r="118" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="23"/>
@@ -2531,6 +2507,9 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A6:B21">

</xml_diff>

<commit_message>
added double crosshairs with shortcut CD (crosshair double)
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F17B4F-03D5-2A45-98C3-1B8DE106E349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87591D2F-12A4-0840-B11E-FDB4061F56D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1520" windowWidth="25600" windowHeight="15520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="1520" windowWidth="25720" windowHeight="25400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="221">
   <si>
     <t>Shortcut</t>
   </si>
@@ -368,9 +368,6 @@
     <t>SA</t>
   </si>
   <si>
-    <t>LT</t>
-  </si>
-  <si>
     <t>LS</t>
   </si>
   <si>
@@ -578,19 +575,10 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Flip X-Y Axis</t>
-  </si>
-  <si>
     <t>XY</t>
   </si>
   <si>
-    <t>Flip X-Z Axis</t>
-  </si>
-  <si>
     <t>XZ</t>
-  </si>
-  <si>
-    <t>Flip Y-Z Axis</t>
   </si>
   <si>
     <t>YZ</t>
@@ -654,12 +642,6 @@
     <t>Zoom out of Spectrum</t>
   </si>
   <si>
-    <t>TA</t>
-  </si>
-  <si>
-    <t>Toggle Share Y Axis Across Display</t>
-  </si>
-  <si>
     <t>ZR</t>
   </si>
   <si>
@@ -784,6 +766,30 @@
   </si>
   <si>
     <t>Ctrl/Cmd+,</t>
+  </si>
+  <si>
+    <t>Toggle Double Crosshairs</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH </t>
+  </si>
+  <si>
+    <t>Toggle Share Last Axis Across Display</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Copy with X-Z Axes Flipped</t>
+  </si>
+  <si>
+    <t>Copy with X-Y Axes Flipped</t>
+  </si>
+  <si>
+    <t>Copy with Y-Z Axes Flipped</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1093,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1475,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,11 +1497,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1503,7 +1509,7 @@
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1613,12 +1619,12 @@
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -1626,10 +1632,10 @@
     </row>
     <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1671,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1690,829 +1696,840 @@
     </row>
     <row r="28" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="C28" s="29" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="C29" s="29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>52</v>
+        <v>213</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>182</v>
+        <v>214</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>110</v>
+      <c r="C34" s="15" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>127</v>
+        <v>113</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="C39" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>54</v>
+        <v>126</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>123</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>132</v>
+        <v>123</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>172</v>
+        <v>139</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="18"/>
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="28"/>
-    </row>
-    <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>167</v>
-      </c>
+      <c r="B56" s="28"/>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="B58" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="8"/>
+      <c r="B67" s="15" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="68" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="18"/>
+      <c r="B68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B68" s="8"/>
-    </row>
-    <row r="69" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C69" s="29" t="s">
-        <v>19</v>
-      </c>
+      <c r="B69" s="8"/>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="B70" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="29" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
-        <v>20</v>
+      <c r="A71" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>115</v>
+        <v>19</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="C73" s="29" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="C74" s="29" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="C75" s="29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B77" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B77" s="15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="8"/>
+      <c r="B78" s="15" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="24" t="s">
+      <c r="A79" s="18"/>
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B79" s="8"/>
-    </row>
-    <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17" t="s">
+      <c r="B80" s="8"/>
+    </row>
+    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B80" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24" t="s">
+      <c r="B81" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+    </row>
+    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B82" s="8"/>
-    </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="B83" s="8"/>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E84" s="16"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>91</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E85" s="16"/>
     </row>
     <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="8"/>
     </row>
     <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="24" t="s">
+      <c r="A90" s="18"/>
+      <c r="B90" s="8"/>
+    </row>
+    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="8"/>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="B91" s="8"/>
     </row>
     <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>139</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B101" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="22" t="s">
+      <c r="B102" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B102" s="15"/>
-    </row>
-    <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="B103" s="15"/>
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C104" s="29" t="s">
-        <v>192</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C105" s="15"/>
+        <v>121</v>
+      </c>
+      <c r="C105" s="29" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C106" s="15"/>
     </row>
     <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>203</v>
+        <v>125</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C107" s="15"/>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C108" s="29" t="s">
-        <v>187</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C108" s="15"/>
     </row>
     <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C109" s="29" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C111" s="29" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="17"/>
-      <c r="B113" s="15"/>
-    </row>
-    <row r="114" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C113" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="17"/>
+      <c r="B114" s="15"/>
+    </row>
+    <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B114" s="8"/>
-    </row>
-    <row r="115" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="20" t="s">
-        <v>46</v>
+      <c r="B115" s="8"/>
+    </row>
+    <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="14" t="s">
+        <v>158</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="23"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="23"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="23"/>
     </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="23"/>
+    </row>
   </sheetData>
-  <sortState ref="A6:B21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">
     <sortCondition ref="A6:A21"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added EN shortcut (estimate noise) to the list
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD05652-0E7D-4347-929D-174662FB3830}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891349C8-8AF7-1343-8BD9-9E87A54C9598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="1100" windowWidth="25720" windowHeight="25400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$122</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$123</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="228">
   <si>
     <t>Shortcut</t>
   </si>
@@ -808,6 +808,12 @@
   </si>
   <si>
     <t xml:space="preserve">      (and Hide Current)</t>
+  </si>
+  <si>
+    <t>Estimate Noise</t>
+  </si>
+  <si>
+    <t>EN</t>
   </si>
 </sst>
 </file>
@@ -1499,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2510,29 +2516,30 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="17"/>
-      <c r="B117" s="15"/>
+      <c r="A117" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C117" s="29"/>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="24" t="s">
+      <c r="A118" s="17"/>
+      <c r="B118" s="15"/>
+    </row>
+    <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B118" s="8"/>
-    </row>
-    <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="14" t="s">
+      <c r="B119" s="8"/>
+    </row>
+    <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B120" s="15" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2540,7 +2547,7 @@
         <v>46</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2548,11 +2555,16 @@
         <v>46</v>
       </c>
       <c r="B122" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B123" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="23"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
@@ -2577,6 +2589,9 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">

</xml_diff>

<commit_message>
Added Zoom shortcuts and moved RI to correct category
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD05652-0E7D-4347-929D-174662FB3830}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1100" windowWidth="25720" windowHeight="25400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$122</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$126</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="237">
   <si>
     <t>Shortcut</t>
   </si>
@@ -338,9 +332,6 @@
     <t>Save as</t>
   </si>
   <si>
-    <t>Pan</t>
-  </si>
-  <si>
     <t>Left click</t>
   </si>
   <si>
@@ -792,12 +783,6 @@
     <t>ZA</t>
   </si>
   <si>
-    <t>ZO, ZS, ZR, ZA</t>
-  </si>
-  <si>
-    <t>ZI, ZS, ZR, ZA</t>
-  </si>
-  <si>
     <t>ZI, ZO, ZR, ZA</t>
   </si>
   <si>
@@ -808,12 +793,54 @@
   </si>
   <si>
     <t xml:space="preserve">      (and Hide Current)</t>
+  </si>
+  <si>
+    <t>Pan / move spectrum around</t>
+  </si>
+  <si>
+    <t>ZP</t>
+  </si>
+  <si>
+    <t>ZN</t>
+  </si>
+  <si>
+    <t>ZO, ZA</t>
+  </si>
+  <si>
+    <t>Store Zoom setting</t>
+  </si>
+  <si>
+    <t>ZR, ZP, ZN, ZA</t>
+  </si>
+  <si>
+    <t>ZS, ZP, ZN, ZA</t>
+  </si>
+  <si>
+    <t>ZP, ZS, ZR, ZA</t>
+  </si>
+  <si>
+    <t>ZN, ZS, ZR, ZA</t>
+  </si>
+  <si>
+    <t>ZI, ZA</t>
+  </si>
+  <si>
+    <t>ZI, ZO</t>
+  </si>
+  <si>
+    <t>Go to next Zoom level</t>
+  </si>
+  <si>
+    <t>Go to previous Zoom level</t>
+  </si>
+  <si>
+    <t>Restore stored Zoom setting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -982,9 +1009,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1118,7 +1147,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="46">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1140,6 +1169,7 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1162,6 +1192,7 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1498,14 +1529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" style="2" customWidth="1"/>
@@ -1514,45 +1545,45 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" thickTop="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" customHeight="1">
       <c r="A7" s="25" t="s">
         <v>22</v>
       </c>
@@ -1560,7 +1591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>31</v>
       </c>
@@ -1568,31 +1599,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17" customHeight="1">
       <c r="A9" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" ht="17" customHeight="1">
       <c r="A11" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" customHeight="1">
       <c r="A12" s="25" t="s">
         <v>33</v>
       </c>
@@ -1600,7 +1631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17" customHeight="1">
       <c r="A13" s="25" t="s">
         <v>4</v>
       </c>
@@ -1608,7 +1639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17" customHeight="1">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>
@@ -1616,7 +1647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17" customHeight="1">
       <c r="A15" s="25" t="s">
         <v>5</v>
       </c>
@@ -1624,7 +1655,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" customHeight="1">
       <c r="A16" s="26" t="s">
         <v>63</v>
       </c>
@@ -1632,31 +1663,31 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -1664,7 +1695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1672,22 +1703,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="21" thickBot="1">
       <c r="A23" s="13" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17" thickTop="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="7" t="s">
         <v>67</v>
       </c>
@@ -1695,16 +1726,16 @@
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="17" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
@@ -1712,150 +1743,150 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" customHeight="1">
       <c r="A28" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="C28" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" customHeight="1">
+      <c r="A29" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="B29" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="17" customHeight="1">
       <c r="A30" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="C30" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="15" t="s">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="B34" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="17" customHeight="1">
       <c r="A35" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" customHeight="1">
+      <c r="A36" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="B36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" customHeight="1">
+      <c r="A37" s="17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="B37" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="C37" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" customHeight="1">
+      <c r="A38" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+      <c r="B38" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="C38" s="29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" customHeight="1">
+      <c r="A40" s="17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+      <c r="B40" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:3" ht="17" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>55</v>
       </c>
@@ -1863,7 +1894,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="17" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>65</v>
       </c>
@@ -1871,715 +1902,759 @@
         <v>66</v>
       </c>
       <c r="C42" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" customHeight="1">
+      <c r="A43" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" customHeight="1">
+      <c r="A44" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" customHeight="1">
+      <c r="A45" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" customHeight="1">
+      <c r="A46" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" customHeight="1">
+      <c r="A47" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" customHeight="1">
+      <c r="A48" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" customHeight="1">
+      <c r="A49" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" customHeight="1">
+      <c r="A50" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" customHeight="1">
+      <c r="A51" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" customHeight="1">
+      <c r="A52" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" customHeight="1">
+      <c r="A53" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" customHeight="1">
+      <c r="A54" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" customHeight="1">
+      <c r="A55" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" customHeight="1">
+      <c r="A56" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" customHeight="1">
+      <c r="A57" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C57" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" customHeight="1">
+      <c r="A58" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" customHeight="1">
+      <c r="A59" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" customHeight="1">
+      <c r="A60" s="18"/>
+      <c r="B60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" ht="17" customHeight="1">
+      <c r="A61" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="28"/>
+    </row>
+    <row r="62" spans="1:3" ht="17" customHeight="1">
+      <c r="A62" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" customHeight="1">
+      <c r="A63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" customHeight="1">
+      <c r="A64" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" customHeight="1">
+      <c r="A65" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" customHeight="1">
+      <c r="A66" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" customHeight="1">
+      <c r="A67" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" customHeight="1">
+      <c r="A68" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" customHeight="1">
+      <c r="A69" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" customHeight="1">
+      <c r="A70" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A71" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A72" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A73" s="18"/>
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A74" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" ht="17" customHeight="1">
+      <c r="A75" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" customHeight="1">
+      <c r="A76" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" customHeight="1">
+      <c r="A77" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" customHeight="1">
+      <c r="A78" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C78" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" customHeight="1">
+      <c r="A79" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" customHeight="1">
+      <c r="A80" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="17" customHeight="1">
+      <c r="A81" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1">
+      <c r="A82" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14">
+      <c r="A83" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" customHeight="1">
+      <c r="A84" s="18"/>
+      <c r="B84" s="8"/>
+    </row>
+    <row r="85" spans="1:5" ht="17" customHeight="1">
+      <c r="A85" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B85" s="8"/>
+    </row>
+    <row r="86" spans="1:5" ht="17" customHeight="1">
+      <c r="A86" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" customHeight="1">
+      <c r="A87" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1">
+      <c r="A89" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" spans="1:5" ht="17" customHeight="1">
+      <c r="A90" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" customHeight="1">
+      <c r="A91" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" s="16"/>
+    </row>
+    <row r="92" spans="1:5" ht="17" customHeight="1">
+      <c r="A92" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1">
+      <c r="A94" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" customHeight="1">
+      <c r="A95" s="18"/>
+      <c r="B95" s="8"/>
+    </row>
+    <row r="96" spans="1:5" ht="17" customHeight="1">
+      <c r="A96" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" s="8"/>
+    </row>
+    <row r="97" spans="1:3" ht="17" customHeight="1">
+      <c r="A97" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" customHeight="1">
+      <c r="A98" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17" customHeight="1">
+      <c r="A99" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B99" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17" customHeight="1">
+      <c r="A100" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" customHeight="1">
+      <c r="A101" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" customHeight="1">
+      <c r="A102" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" customHeight="1">
+      <c r="A103" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" customHeight="1">
+      <c r="A104" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17" customHeight="1">
+      <c r="A105" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17" customHeight="1">
+      <c r="A106" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17" customHeight="1">
+      <c r="A107" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" customHeight="1">
+      <c r="A108" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" s="15"/>
+    </row>
+    <row r="109" spans="1:3" ht="17" customHeight="1">
+      <c r="A109" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" customHeight="1">
+      <c r="A110" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17" customHeight="1">
+      <c r="A111" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17" customHeight="1">
+      <c r="A112" s="17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="29" t="s">
+      <c r="B112" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C112" s="15"/>
+    </row>
+    <row r="113" spans="1:3" ht="17" customHeight="1">
+      <c r="A113" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B113" s="15" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="29" t="s">
+      <c r="C113" s="15"/>
+    </row>
+    <row r="114" spans="1:3" ht="17" customHeight="1">
+      <c r="A114" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B114" s="15"/>
+      <c r="C114" s="15"/>
+    </row>
+    <row r="115" spans="1:3" ht="17" customHeight="1">
+      <c r="A115" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C115" s="15"/>
+    </row>
+    <row r="116" spans="1:3" ht="17" customHeight="1">
+      <c r="A116" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C116" s="29" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" customHeight="1">
+      <c r="A117" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C117" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" customHeight="1">
+      <c r="A118" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" s="29" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="C52" s="29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B53" s="15" t="s">
+    <row r="119" spans="1:3" ht="17" customHeight="1">
+      <c r="A119" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="C53" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="8"/>
-    </row>
-    <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="28"/>
-    </row>
-    <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="8"/>
-    </row>
-    <row r="70" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" s="8"/>
-    </row>
-    <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C74" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C75" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C76" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C77" s="29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="8"/>
-    </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="23"/>
-      <c r="B83" s="23"/>
-    </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B84" s="8"/>
-    </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E86" s="16"/>
-    </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
-      <c r="B91" s="8"/>
-    </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B92" s="8"/>
-    </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B97" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B99" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B104" s="15"/>
-    </row>
-    <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B105" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B106" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C107" s="29" t="s">
+      <c r="B119" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C119" s="29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" customHeight="1">
+      <c r="A120" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" s="29" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B108" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="C108" s="15"/>
-    </row>
-    <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C109" s="15"/>
-    </row>
-    <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B110" s="15"/>
-      <c r="C110" s="15"/>
-    </row>
-    <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C111" s="15"/>
-    </row>
-    <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C112" s="29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="B113" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C113" s="29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C114" s="29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C115" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B116" s="15" t="s">
+    <row r="121" spans="1:3" ht="17" customHeight="1">
+      <c r="A121" s="17"/>
+      <c r="B121" s="15"/>
+    </row>
+    <row r="122" spans="1:3" ht="17" customHeight="1">
+      <c r="A122" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B122" s="8"/>
+    </row>
+    <row r="123" spans="1:3" ht="17" customHeight="1">
+      <c r="A123" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C116" s="29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="17"/>
-      <c r="B117" s="15"/>
-    </row>
-    <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B118" s="8"/>
-    </row>
-    <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="14" t="s">
+      <c r="B123" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B119" s="15" t="s">
+    </row>
+    <row r="124" spans="1:3" ht="17" customHeight="1">
+      <c r="A124" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17" customHeight="1">
+      <c r="A125" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17" customHeight="1">
+      <c r="A126" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B126" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="23"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="23"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="23"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="23"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3">
       <c r="A127" s="23"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3">
       <c r="A128" s="23"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="23"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="23"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="23"/>
     </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="23"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="23"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="23"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="23"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">
+  <sortState ref="A6:B21">
     <sortCondition ref="A6:A21"/>
   </sortState>
   <mergeCells count="1">
@@ -2588,5 +2663,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.57000000000000006" right="0.25" top="0.35629921259842523" bottom="0.15944881889763785" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zoom/pan now work on current strip to match all zoom functions TU/TD now work instantly on active trace (trace immediately under cursor) fixed double cursor again (silly new error) fixed bug for printing - colours are now uppercase added TabZ to shortcuts
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E657E-AAF3-7E4D-BE53-03A12043094B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3AD209-EC5F-7146-8E86-BAB3A83EDDD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$127</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$128</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="242">
   <si>
     <t>Shortcut</t>
   </si>
@@ -657,12 +657,6 @@
     <t>TV, TU, TD</t>
   </si>
   <si>
-    <t>PC, PT, TR</t>
-  </si>
-  <si>
-    <t>PC, PV, PT</t>
-  </si>
-  <si>
     <t>XZ, YZ</t>
   </si>
   <si>
@@ -672,9 +666,6 @@
     <t>PC, PV, TR</t>
   </si>
   <si>
-    <t>PV, PT, TR</t>
-  </si>
-  <si>
     <t>XY, XZ</t>
   </si>
   <si>
@@ -705,9 +696,6 @@
     <t>TabQ</t>
   </si>
   <si>
-    <t>Toggle all Spectra on Current Display</t>
-  </si>
-  <si>
     <t>TabA</t>
   </si>
   <si>
@@ -847,6 +835,27 @@
   </si>
   <si>
     <t>EN</t>
+  </si>
+  <si>
+    <t>PV, TA, TR</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>PC, TA, TR</t>
+  </si>
+  <si>
+    <t>PC, PV, TA+C112</t>
+  </si>
+  <si>
+    <t>Show all Spectra on Current Display</t>
+  </si>
+  <si>
+    <t>TabZ</t>
+  </si>
+  <si>
+    <t>Hide all Spectra on Current Display</t>
   </si>
 </sst>
 </file>
@@ -1542,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1559,7 +1568,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1589,7 +1598,7 @@
     </row>
     <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -1763,7 +1772,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1774,18 +1783,18 @@
         <v>104</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1807,7 +1816,7 @@
         <v>119</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1818,7 +1827,7 @@
         <v>115</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1829,7 +1838,7 @@
         <v>117</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,7 +1934,7 @@
         <v>122</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1938,13 +1947,13 @@
     </row>
     <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>130</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>175</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1960,10 +1969,10 @@
         <v>133</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1974,7 +1983,7 @@
         <v>137</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>176</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1990,10 +1999,10 @@
         <v>167</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2001,98 +2010,98 @@
         <v>168</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>171</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>169</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2166,7 +2175,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2179,10 +2188,10 @@
     </row>
     <row r="71" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2290,7 +2299,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2438,7 +2447,7 @@
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>100</v>
@@ -2465,7 +2474,7 @@
         <v>43</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2482,15 +2491,15 @@
         <v>59</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>59</v>
@@ -2504,7 +2513,7 @@
         <v>120</v>
       </c>
       <c r="C111" s="29" t="s">
-        <v>180</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2512,123 +2521,132 @@
         <v>123</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C112" s="15"/>
+        <v>189</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="C113" s="15"/>
+        <v>187</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
     </row>
     <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="C115" s="15"/>
+        <v>188</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C116" s="29" t="s">
-        <v>219</v>
+        <v>240</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="C121" s="29"/>
+        <v>155</v>
+      </c>
+      <c r="C121" s="29" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="17"/>
-      <c r="B122" s="15"/>
+      <c r="A122" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C122" s="29"/>
     </row>
     <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="24" t="s">
+      <c r="A123" s="17"/>
+      <c r="B123" s="15"/>
+    </row>
+    <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B123" s="8"/>
-    </row>
-    <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="14" t="s">
+      <c r="B124" s="8"/>
+    </row>
+    <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B124" s="15" t="s">
+      <c r="B125" s="15" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B125" s="15" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2636,7 +2654,7 @@
         <v>46</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2644,11 +2662,16 @@
         <v>46</v>
       </c>
       <c r="B127" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B128" s="15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="23"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="23"/>
@@ -2673,6 +2696,9 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">

</xml_diff>

<commit_message>
spelling mistake in shortcuts
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3AD209-EC5F-7146-8E86-BAB3A83EDDD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34CF6D-6F42-4B44-BE38-C07C51BEC8D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$128</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$126</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="238">
   <si>
     <t>Shortcut</t>
   </si>
@@ -642,15 +642,9 @@
     <t>ZR</t>
   </si>
   <si>
-    <t>Store Zoom</t>
-  </si>
-  <si>
     <t>ZS</t>
   </si>
   <si>
-    <t>Restore Zoom</t>
-  </si>
-  <si>
     <t>Related</t>
   </si>
   <si>
@@ -777,12 +771,6 @@
     <t>ZA</t>
   </si>
   <si>
-    <t>ZI, ZO, ZR, ZA</t>
-  </si>
-  <si>
-    <t>ZI, ZO, ZS, ZA</t>
-  </si>
-  <si>
     <t>Move to Previous Spectrum</t>
   </si>
   <si>
@@ -846,9 +834,6 @@
     <t>PC, TA, TR</t>
   </si>
   <si>
-    <t>PC, PV, TA+C112</t>
-  </si>
-  <si>
     <t>Show all Spectra on Current Display</t>
   </si>
   <si>
@@ -856,6 +841,9 @@
   </si>
   <si>
     <t>Hide all Spectra on Current Display</t>
+  </si>
+  <si>
+    <t>PC, PV, TA</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1568,7 +1556,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1598,7 +1586,7 @@
     </row>
     <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -1747,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1772,7 +1760,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1783,18 +1771,18 @@
         <v>104</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>203</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1805,7 +1793,7 @@
         <v>118</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1816,7 +1804,7 @@
         <v>119</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1827,7 +1815,7 @@
         <v>115</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1838,7 +1826,7 @@
         <v>117</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1934,7 +1922,7 @@
         <v>122</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1947,13 +1935,13 @@
     </row>
     <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>130</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1969,10 +1957,10 @@
         <v>133</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1983,7 +1971,7 @@
         <v>137</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1999,10 +1987,10 @@
         <v>167</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2010,98 +1998,98 @@
         <v>168</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>169</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>190</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2175,7 +2163,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2188,10 +2176,10 @@
     </row>
     <row r="71" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2299,7 +2287,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2447,7 +2435,7 @@
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>100</v>
@@ -2474,7 +2462,7 @@
         <v>43</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2491,15 +2479,15 @@
         <v>59</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>59</v>
@@ -2513,7 +2501,7 @@
         <v>120</v>
       </c>
       <c r="C111" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2521,132 +2509,126 @@
         <v>123</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B113" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
     </row>
     <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C120" s="29" t="s">
-        <v>176</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="C120" s="29"/>
     </row>
     <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C121" s="29" t="s">
-        <v>178</v>
-      </c>
+      <c r="A121" s="17"/>
+      <c r="B121" s="15"/>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C122" s="29"/>
+      <c r="A122" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B122" s="8"/>
     </row>
     <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="17"/>
-      <c r="B123" s="15"/>
+      <c r="A123" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B124" s="8"/>
+      <c r="A124" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="14" t="s">
-        <v>156</v>
+      <c r="A125" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2654,24 +2636,14 @@
         <v>46</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B127" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B128" s="15" t="s">
         <v>158</v>
       </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="23"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="23"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="23"/>
@@ -2693,12 +2665,6 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="23"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">

</xml_diff>

<commit_message>
added stack shortcut SK and to shortcuts pdf
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34CF6D-6F42-4B44-BE38-C07C51BEC8D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51286E40-33A1-444C-810D-670CBDF594E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$126</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$127</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="240">
   <si>
     <t>Shortcut</t>
   </si>
@@ -844,6 +844,12 @@
   </si>
   <si>
     <t>PC, PV, TA</t>
+  </si>
+  <si>
+    <t>Stack 1D spectra</t>
+  </si>
+  <si>
+    <t>SK</t>
   </si>
 </sst>
 </file>
@@ -1539,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,651 +1982,652 @@
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>166</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C49" s="29"/>
     </row>
     <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C60" s="29" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="8"/>
-    </row>
     <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="18"/>
+      <c r="B61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="28"/>
-    </row>
-    <row r="62" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>161</v>
-      </c>
+      <c r="B62" s="28"/>
     </row>
     <row r="63" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B64" s="15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
+    <row r="65" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>196</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B73" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="8"/>
-    </row>
     <row r="74" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="21" t="s">
+      <c r="A74" s="18"/>
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B74" s="8"/>
-    </row>
-    <row r="75" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="29" t="s">
-        <v>19</v>
-      </c>
+      <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B77" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="29" t="s">
+      <c r="C77" s="29" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C78" s="29" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B79" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" s="29" t="s">
         <v>86</v>
-      </c>
-      <c r="C79" s="29" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B81" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="C81" s="29" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B83" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B84" s="15" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
-      <c r="B84" s="8"/>
-    </row>
     <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="18"/>
+      <c r="B85" s="8"/>
+    </row>
+    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B85" s="8"/>
-    </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="14" t="s">
+      <c r="B86" s="8"/>
+    </row>
+    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B87" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="17" t="s">
+    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B88" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="23"/>
-      <c r="B88" s="23"/>
-    </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="24" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
+    </row>
+    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="8"/>
-    </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E91" s="16"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>89</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E92" s="16"/>
     </row>
     <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B95" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="8"/>
-    </row>
     <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24" t="s">
+      <c r="A96" s="18"/>
+      <c r="B96" s="8"/>
+    </row>
+    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B96" s="8"/>
-    </row>
-    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B97" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="B97" s="8"/>
     </row>
     <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B108" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="22" t="s">
+    <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B108" s="15"/>
-    </row>
-    <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>210</v>
-      </c>
+      <c r="B109" s="15"/>
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>209</v>
+        <v>62</v>
       </c>
       <c r="B110" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" s="15" t="s">
         <v>210</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C111" s="29" t="s">
-        <v>231</v>
+        <v>210</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>185</v>
+        <v>120</v>
+      </c>
+      <c r="C112" s="29" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="B113" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C113" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
+        <v>213</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>235</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B115" s="15"/>
+      <c r="C115" s="15"/>
     </row>
     <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B116" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C117" s="29" t="s">
-        <v>173</v>
+        <v>235</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B121" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="C120" s="29"/>
-    </row>
-    <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="17"/>
-      <c r="B121" s="15"/>
+      <c r="C121" s="29"/>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="24" t="s">
+      <c r="A122" s="17"/>
+      <c r="B122" s="15"/>
+    </row>
+    <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B122" s="8"/>
-    </row>
-    <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="14" t="s">
+      <c r="B123" s="8"/>
+    </row>
+    <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B124" s="15" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B124" s="15" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2628,7 +2635,7 @@
         <v>46</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2636,11 +2643,16 @@
         <v>46</v>
       </c>
       <c r="B126" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B127" s="15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="23"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
@@ -2665,6 +2677,9 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">

</xml_diff>

<commit_message>
implementing peak volumes - function added to peakList and peakUtils added option to preferences added shortcut 'ev' to pdf changed labelling in pickAndAssign
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969CAE40-AEC9-9044-9ED6-1D1AF95CEC28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EBB4E5-5351-3748-B328-EA1B4E813CE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11020" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$128</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$129</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="244">
   <si>
     <t>Shortcut</t>
   </si>
@@ -856,6 +856,12 @@
   </si>
   <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Estimate Volumes</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2306,351 +2312,352 @@
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C84" s="29"/>
+    </row>
+    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B85" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B86" s="15" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="8"/>
-    </row>
     <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24" t="s">
+      <c r="A87" s="18"/>
+      <c r="B87" s="8"/>
+    </row>
+    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B87" s="8"/>
-    </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="14" t="s">
+      <c r="B88" s="8"/>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B89" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
+    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B90" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="23"/>
-      <c r="B90" s="23"/>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+    </row>
+    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B91" s="8"/>
-    </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="B92" s="8"/>
     </row>
     <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E93" s="16"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>89</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E94" s="16"/>
     </row>
     <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B97" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="18"/>
-      <c r="B97" s="8"/>
-    </row>
     <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="24" t="s">
+      <c r="A98" s="18"/>
+      <c r="B98" s="8"/>
+    </row>
+    <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B98" s="8"/>
-    </row>
-    <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B99" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="B99" s="8"/>
     </row>
     <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B110" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="22" t="s">
+    <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B110" s="15"/>
-    </row>
-    <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>210</v>
-      </c>
+      <c r="B111" s="15"/>
     </row>
     <row r="112" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>209</v>
+        <v>62</v>
       </c>
       <c r="B112" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C112" s="15" t="s">
         <v>210</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C113" s="29" t="s">
-        <v>231</v>
+        <v>210</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>185</v>
+        <v>120</v>
+      </c>
+      <c r="C114" s="29" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="B115" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C115" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B116" s="15"/>
-      <c r="C116" s="15"/>
+        <v>213</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>235</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B117" s="15"/>
+      <c r="C117" s="15"/>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B118" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C119" s="29" t="s">
-        <v>173</v>
+        <v>235</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C121" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C122" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B123" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="C122" s="29"/>
-    </row>
-    <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="17"/>
-      <c r="B123" s="15"/>
+      <c r="C123" s="29"/>
     </row>
     <row r="124" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="24" t="s">
+      <c r="A124" s="17"/>
+      <c r="B124" s="15"/>
+    </row>
+    <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B124" s="8"/>
-    </row>
-    <row r="125" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="14" t="s">
+      <c r="B125" s="8"/>
+    </row>
+    <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B125" s="15" t="s">
+      <c r="B126" s="15" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2658,7 +2665,7 @@
         <v>46</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2666,35 +2673,43 @@
         <v>46</v>
       </c>
       <c r="B128" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B129" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="23"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="23"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="23"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="23"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="23"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B21">

</xml_diff>

<commit_message>
updated shortcuts for peakAssigner (AP) and NmrAtomAssigner (AN)
</commit_message>
<xml_diff>
--- a/doc/static/AnalysisShortcuts.xlsx
+++ b/doc/static/AnalysisShortcuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejb66/PycharmProjects/Git/AnalysisV3/doc/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EBB4E5-5351-3748-B328-EA1B4E813CE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50B739C-D108-8D4B-A6D3-1067C61E8771}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26840" yWindow="460" windowWidth="18900" windowHeight="27980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,12 +410,6 @@
     <t>RC</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
     <t>Toggle Grid</t>
   </si>
   <si>
@@ -714,9 +708,6 @@
     <t>ZO or -</t>
   </si>
   <si>
-    <t>Atom Assigner</t>
-  </si>
-  <si>
     <t>Space-Space</t>
   </si>
   <si>
@@ -862,6 +853,15 @@
   </si>
   <si>
     <t>Estimate Volumes</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NmrAtom Assigner </t>
   </si>
 </sst>
 </file>
@@ -1559,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,7 +1574,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1772,35 +1772,35 @@
     </row>
     <row r="28" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1808,10 +1808,10 @@
         <v>52</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1819,98 +1819,98 @@
         <v>53</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>106</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B37" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>110</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B40" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1929,202 +1929,202 @@
         <v>66</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>137</v>
-      </c>
       <c r="C48" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C49" s="29"/>
     </row>
     <row r="50" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" s="29" t="s">
         <v>188</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C61" s="29"/>
     </row>
@@ -2143,7 +2143,7 @@
         <v>72</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2151,7 +2151,7 @@
         <v>81</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,7 +2167,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2180,18 +2180,18 @@
     </row>
     <row r="69" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2199,7 +2199,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2212,10 +2212,10 @@
     </row>
     <row r="73" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2223,7 +2223,7 @@
         <v>17</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2249,7 +2249,7 @@
     </row>
     <row r="78" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>19</v>
@@ -2263,15 +2263,15 @@
         <v>20</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C80" s="29" t="s">
         <v>86</v>
@@ -2279,43 +2279,43 @@
     </row>
     <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B81" s="15" t="s">
         <v>86</v>
       </c>
       <c r="C81" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B83" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="C83" s="29" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C84" s="29"/>
     </row>
@@ -2332,7 +2332,7 @@
         <v>35</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2401,94 +2401,94 @@
         <v>29</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>99</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B98" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="8"/>
-    </row>
     <row r="99" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="24" t="s">
+      <c r="A99" s="18"/>
+      <c r="B99" s="8"/>
+    </row>
+    <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B99" s="8"/>
-    </row>
-    <row r="100" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="B100" s="8"/>
     </row>
     <row r="101" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>27</v>
@@ -2496,10 +2496,10 @@
     </row>
     <row r="109" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2507,7 +2507,7 @@
         <v>43</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2524,15 +2524,15 @@
         <v>59</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C113" s="15" t="s">
         <v>59</v>
@@ -2543,102 +2543,102 @@
         <v>60</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B116" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C116" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
     </row>
     <row r="118" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C121" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C122" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C123" s="29"/>
     </row>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="126" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2665,7 +2665,7 @@
         <v>46</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2673,7 +2673,7 @@
         <v>46</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
         <v>46</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>